<commit_message>
Additional var on strings, xforms extra customizations
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/out_migration_registration.xlsx
+++ b/xforms/xlsforms/out_migration_registration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25605" yWindow="-135" windowWidth="20730" windowHeight="11700" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20430" windowHeight="7905" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="180">
   <si>
     <t>type</t>
   </si>
@@ -550,6 +550,12 @@
   </si>
   <si>
     <t>time_absence</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -1705,13 +1711,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R92"/>
+  <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L11" sqref="L11:L13"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12"/>
@@ -1960,93 +1966,100 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="22.5" customHeight="1">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:18" ht="15" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" ht="22.5" customHeight="1">
+      <c r="A10" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="J9" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="J10" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="32.25" customHeight="1">
+    <row r="11" spans="1:18">
       <c r="A11" s="5" t="s">
-        <v>118</v>
+        <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="J11" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1">
+    <row r="12" spans="1:18" ht="32.25" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J12" s="4" t="b">
         <v>1</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1">
@@ -2054,22 +2067,22 @@
         <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1">
@@ -2077,16 +2090,16 @@
         <v>21</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J14" s="4" t="b">
         <v>1</v>
@@ -2100,16 +2113,16 @@
         <v>21</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J15" s="4" t="b">
         <v>1</v>
@@ -2123,16 +2136,16 @@
         <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J16" s="4" t="b">
         <v>1</v>
@@ -2141,142 +2154,154 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>116</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J17" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="18" customHeight="1">
+      <c r="M17" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>42</v>
+        <v>124</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="J18" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="20.25" customHeight="1">
+    <row r="19" spans="1:14" ht="18" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J19" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="M19" s="5" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="20" spans="1:14" ht="20.25" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
+      <c r="A20" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J20" s="4" t="b">
         <v>1</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="24">
-      <c r="A21" s="5" t="s">
-        <v>85</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="20.25" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="J21" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="M21" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="24">
       <c r="A22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="N22" s="5" t="b">
+      <c r="N23" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="10"/>
@@ -2290,28 +2315,30 @@
       <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="2"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
+      <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="7"/>
-      <c r="B26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="11"/>
+      <c r="B26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="2"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -2319,7 +2346,6 @@
     <row r="28" spans="1:14">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -2335,17 +2361,17 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="11"/>
+      <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="11"/>
+      <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
+      <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="2"/>
@@ -2360,9 +2386,9 @@
     <row r="32" spans="1:14">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="E32" s="11"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2406,7 +2432,6 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="J36" s="3"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="2"/>
@@ -2439,6 +2464,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
+      <c r="J39" s="3"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="2"/>
@@ -2449,19 +2475,26 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="J44" s="3"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="J41" s="3"/>
     </row>
     <row r="45" spans="1:10">
       <c r="J45" s="3"/>
     </row>
-    <row r="53" spans="10:10">
-      <c r="J53" s="3"/>
-    </row>
-    <row r="61" spans="10:10">
-      <c r="J61" s="3"/>
+    <row r="46" spans="1:10">
+      <c r="J46" s="3"/>
+    </row>
+    <row r="54" spans="10:10">
+      <c r="J54" s="3"/>
     </row>
     <row r="62" spans="10:10">
       <c r="J62" s="3"/>
@@ -2475,8 +2508,8 @@
     <row r="65" spans="10:10">
       <c r="J65" s="3"/>
     </row>
-    <row r="82" spans="1:10">
-      <c r="J82" s="3"/>
+    <row r="66" spans="10:10">
+      <c r="J66" s="3"/>
     </row>
     <row r="83" spans="1:10">
       <c r="J83" s="3"/>
@@ -2491,7 +2524,6 @@
       <c r="J86" s="3"/>
     </row>
     <row r="87" spans="1:10">
-      <c r="A87" s="3"/>
       <c r="J87" s="3"/>
     </row>
     <row r="88" spans="1:10">
@@ -2503,10 +2535,14 @@
       <c r="J89" s="3"/>
     </row>
     <row r="90" spans="1:10">
+      <c r="A90" s="3"/>
       <c r="J90" s="3"/>
     </row>
-    <row r="92" spans="1:10">
-      <c r="J92" s="3"/>
+    <row r="91" spans="1:10">
+      <c r="J91" s="3"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="J93" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>